<commit_message>
Updated status as I made another routine
</commit_message>
<xml_diff>
--- a/documentation/API.xlsx
+++ b/documentation/API.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
   <si>
     <t>ACCESSION_SEARCH</t>
   </si>
@@ -244,13 +244,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,7 +523,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -533,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="31.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,7 +560,7 @@
       <c r="E1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>52</v>
       </c>
     </row>
@@ -580,7 +580,7 @@
       <c r="E2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>51</v>
       </c>
     </row>
@@ -698,6 +698,9 @@
         <v>45</v>
       </c>
       <c r="E9" s="2"/>
+      <c r="F9" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -713,36 +716,36 @@
         <v>12</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="3"/>
+      <c r="E11" s="5"/>
       <c r="F11" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
       <c r="D12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="3"/>
+      <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">

</xml_diff>

<commit_message>
Added Highlighting Exon Task observation.
</commit_message>
<xml_diff>
--- a/documentation/API.xlsx
+++ b/documentation/API.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="54">
   <si>
     <t>ACCESSION_SEARCH</t>
   </si>
@@ -96,12 +96,6 @@
     <t>DNA sequence</t>
   </si>
   <si>
-    <t>1 hash and 1 string</t>
-  </si>
-  <si>
-    <t>hash of exons position and string with dna sequence</t>
-  </si>
-  <si>
     <t>Coding sequence and amino acids sequence</t>
   </si>
   <si>
@@ -150,15 +144,9 @@
     <t>INTRON/EXON</t>
   </si>
   <si>
-    <t>hash or array with alternate intron/exons to be then highlighted in the cgi.</t>
-  </si>
-  <si>
     <t>full dna sequence string and hash of exons position</t>
   </si>
   <si>
-    <t>String of the coding DNA (concatenated exons)</t>
-  </si>
-  <si>
     <t>ALL_Protein</t>
   </si>
   <si>
@@ -178,6 +166,21 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>Does not need a function</t>
+  </si>
+  <si>
+    <t>Does not need a function.</t>
+  </si>
+  <si>
+    <t>The coding sequence; concatenated exons (1 string).</t>
+  </si>
+  <si>
+    <t>This task can be completed by only giving the front end the full DNA sequence and an hash of exons positions/length; both retrievable with queries; all the front end needs is to know which sbstring within the main string to highligh; same we decided to do for the restriction sites task.</t>
+  </si>
+  <si>
+    <t>The front end can do this task with 2 lines of code by only having the full DNA sequence and an hash of exons position. We aleady have SQL fnctions retrieving those for the front end to use.  The front end just need to place tags around each exon subtring.</t>
   </si>
 </sst>
 </file>
@@ -523,7 +526,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -533,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="31.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,19 +552,19 @@
         <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -578,27 +581,27 @@
         <v>3</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -606,16 +609,16 @@
         <v>21</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -623,16 +626,16 @@
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -640,16 +643,16 @@
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -657,49 +660,54 @@
         <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="2" t="s">
+    </row>
+    <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="B8" s="2" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E8" s="2"/>
+        <v>53</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -707,7 +715,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>2</v>
@@ -717,7 +725,7 @@
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -725,7 +733,7 @@
         <v>13</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>4</v>
@@ -735,7 +743,7 @@
       </c>
       <c r="E11" s="5"/>
       <c r="F11" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -760,7 +768,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -771,7 +779,7 @@
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>24</v>
@@ -780,7 +788,7 @@
         <v>4</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2 more functions completed
</commit_message>
<xml_diff>
--- a/documentation/API.xlsx
+++ b/documentation/API.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="55">
   <si>
     <t>ACCESSION_SEARCH</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>The front end can do this task with 2 lines of code by only having the full DNA sequence and an hash of exons position. We aleady have SQL fnctions retrieving those for the front end to use.  The front end just need to place tags around each exon subtring.</t>
+  </si>
+  <si>
+    <t>DOne</t>
   </si>
 </sst>
 </file>
@@ -526,7 +529,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -537,7 +540,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="31.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,7 +646,9 @@
       <c r="E5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="3"/>
+      <c r="F5" s="3" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -661,7 +666,9 @@
       <c r="E6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="3"/>
+      <c r="F6" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">

</xml_diff>

<commit_message>
New query function made; updated status.
</commit_message>
<xml_diff>
--- a/documentation/API.xlsx
+++ b/documentation/API.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
   <si>
     <t>ACCESSION_SEARCH</t>
   </si>
@@ -532,7 +532,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -542,7 +542,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -689,6 +689,9 @@
       <c r="E7" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="F7" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">

</xml_diff>